<commit_message>
daat read from testdata excel for XML
</commit_message>
<xml_diff>
--- a/utilities/TestData/MMTestData.xlsx
+++ b/utilities/TestData/MMTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20349"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B9482EC-789A-4F40-B2D1-239C70ED48B5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA8B63FA-431E-4174-AF88-090BD2EA788F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -449,7 +449,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -551,8 +551,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BE77B3C-BA60-4FB7-BD2C-03A43C794ADE}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>